<commit_message>
A wide range of cleanup and fixes for nutrientCalcs. For the xlsx file a fix to the lookup table that had caused misidentification of foods by food group
</commit_message>
<xml_diff>
--- a/data/food commodity to food group table V1.xlsx
+++ b/data/food commodity to food group table V1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="180" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -373,6 +370,9 @@
   </si>
   <si>
     <t>sweeteners</t>
+  </si>
+  <si>
+    <t>IMPACTCode</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -496,10 +496,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -513,6 +509,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -887,16 +886,16 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="12.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="10.83203125" style="11"/>
-    <col min="6" max="6" width="10.83203125" style="9"/>
+    <col min="3" max="3" width="10.83203125" style="9"/>
+    <col min="5" max="5" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="10.83203125" style="7"/>
     <col min="7" max="7" width="10.83203125" style="2"/>
     <col min="8" max="8" width="16.83203125" style="3" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="4"/>
@@ -904,816 +903,816 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="30">
       <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" t="str">
-        <f>VLOOKUP(C2,F$2:F$14,1)</f>
+      <c r="C2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7" t="str">
+        <f>VLOOKUP(C2,E$2:F$14,2)</f>
         <v>fruits</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>111</v>
+      <c r="E2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D47" si="0">VLOOKUP(C3,F$2:F$14,1)</f>
+      <c r="C3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="7" t="str">
+        <f t="shared" ref="D3:D47" si="0">VLOOKUP(C3,E$2:F$14,2)</f>
         <v>cereals</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>96</v>
+      <c r="E3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" t="str">
+      <c r="C4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="7" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>112</v>
+      <c r="E4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>fruits</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>98</v>
+      <c r="C5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>meats</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>beverages</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>beverages</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>113</v>
+      <c r="F6" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>roots</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>roots</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>100</v>
+      <c r="F7" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" t="str">
+      <c r="C8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>101</v>
+      <c r="E8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="30">
       <c r="A9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" t="str">
+      <c r="C9" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>114</v>
+      <c r="E9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" t="str">
+      <c r="C10" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>115</v>
+      <c r="E10" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" t="str">
+      <c r="C11" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>eggs</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>97</v>
+      <c r="E11" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="30">
       <c r="A12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>116</v>
+      <c r="C12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="30">
       <c r="A13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>meats</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>117</v>
+      <c r="C13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oilSeeds</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>fruits</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>102</v>
+      <c r="D14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>meats</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" t="str">
+      <c r="C15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="7" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" t="str">
+      <c r="C16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>cereals</v>
+      <c r="C17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>diary</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" t="str">
+      <c r="C18" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" t="str">
+      <c r="C19" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" t="str">
+      <c r="C20" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="7" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
       <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" t="str">
+      <c r="C21" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" t="str">
+      <c r="C22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="str">
+      <c r="C23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="7" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30">
       <c r="A24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
+      <c r="C24" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" t="str">
+      <c r="C25" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="7" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
+      <c r="C26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>fruits</v>
+      <c r="C27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>meats</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30">
       <c r="A28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" t="str">
+      <c r="C28" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="7" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>fruits</v>
+      <c r="C29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>meats</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" t="str">
+      <c r="C30" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30">
       <c r="A31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
+      <c r="C31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>meats</v>
+      <c r="C32" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oilSeeds</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30">
       <c r="A33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
+      <c r="C33" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
       <c r="A34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
+      <c r="C34" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>meats</v>
+      <c r="C35" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oilSeeds</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" t="str">
+      <c r="C36" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>meats</v>
+      <c r="C37" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oilSeeds</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30">
       <c r="A38" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D38" t="str">
+      <c r="C38" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="7" t="str">
         <f t="shared" si="0"/>
         <v>fruits</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>roots</v>
+      <c r="C39" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>sweeteners</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30">
       <c r="A40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" t="str">
+      <c r="C40" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="7" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30">
       <c r="A41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" t="str">
+      <c r="C41" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="7" t="str">
         <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" t="str">
+      <c r="C42" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="7" t="str">
         <f t="shared" si="0"/>
         <v>fruits</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30">
       <c r="A43" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>meats</v>
+      <c r="C43" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oilSeeds</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30">
       <c r="A44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>eggs</v>
+      <c r="C44" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>oils</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" t="str">
+      <c r="C45" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="7" t="str">
         <f t="shared" si="0"/>
         <v>vegetables</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" t="str">
+      <c r="C46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="7" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30">
       <c r="A47" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" t="str">
+      <c r="C47" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="7" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>

</xml_diff>

<commit_message>
A lot of changes since the previous commit.
</commit_message>
<xml_diff>
--- a/data/food commodity to food group table V1.xlsx
+++ b/data/food commodity to food group table V1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1980" yWindow="3820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -485,12 +485,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -883,879 +882,865 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="9"/>
-    <col min="5" max="5" width="10.83203125" style="9"/>
-    <col min="6" max="6" width="10.83203125" style="7"/>
-    <col min="7" max="7" width="10.83203125" style="2"/>
-    <col min="8" max="8" width="16.83203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="30">
-      <c r="A2" s="5" t="s">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="30">
+      <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" s="6" t="str">
         <f>VLOOKUP(C2,E$2:F$14,2)</f>
         <v>fruits</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="7" t="str">
+      <c r="D3" s="6" t="str">
         <f t="shared" ref="D3:D47" si="0">VLOOKUP(C3,E$2:F$14,2)</f>
         <v>cereals</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="7" t="str">
+      <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="7" t="str">
+      <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>meats</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="5" t="s">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="7" t="str">
+      <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="5" t="s">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="7" t="str">
+      <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="5" t="s">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="7" t="str">
+      <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="5" t="s">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="7" t="str">
+      <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="5" t="s">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="7" t="str">
+      <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="5" t="s">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="7" t="str">
+      <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>eggs</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="5" t="s">
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="7" t="str">
+      <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="30">
-      <c r="A13" s="5" t="s">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="7" t="str">
+      <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="7" t="str">
+      <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>meats</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="5" t="s">
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="7" t="str">
+      <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="7" t="str">
+      <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="7" t="str">
+      <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>diary</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="7" t="str">
+      <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="7" t="str">
+      <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="7" t="str">
+      <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="7" t="str">
+      <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="7" t="str">
+      <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>pulses</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="7" t="str">
+      <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="7" t="str">
+      <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="7" t="str">
+      <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="7" t="str">
+      <c r="D27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>meats</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30">
-      <c r="A28" s="5" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="7" t="str">
+      <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="7" t="str">
+      <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>meats</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="7" t="str">
+      <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="7" t="str">
+      <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="7" t="str">
+      <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30">
-      <c r="A33" s="5" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="7" t="str">
+      <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="7" t="str">
+      <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="7" t="str">
+      <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="7" t="str">
+      <c r="D36" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="7" t="str">
+      <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D38" s="7" t="str">
+      <c r="D38" s="6" t="str">
         <f t="shared" si="0"/>
         <v>fruits</v>
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="7" t="str">
+      <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>sweeteners</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="7" t="str">
+      <c r="D40" s="6" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="7" t="str">
+      <c r="D41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>beverages</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="7" t="str">
+      <c r="D42" s="6" t="str">
         <f t="shared" si="0"/>
         <v>fruits</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="7" t="str">
+      <c r="D43" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oilSeeds</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:4">
+      <c r="A44" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D44" s="7" t="str">
+      <c r="D44" s="6" t="str">
         <f t="shared" si="0"/>
         <v>oils</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="7" t="str">
+      <c r="D45" s="6" t="str">
         <f t="shared" si="0"/>
         <v>vegetables</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D46" s="7" t="str">
+      <c r="D46" s="6" t="str">
         <f t="shared" si="0"/>
         <v>cereals</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:4">
+      <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="7" t="str">
+      <c r="D47" s="6" t="str">
         <f t="shared" si="0"/>
         <v>roots</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
     </row>
   </sheetData>
   <sortState ref="A2:B79">

</xml_diff>